<commit_message>
a little refactoring of q-learner
</commit_message>
<xml_diff>
--- a/frozenlake_vis.xlsx
+++ b/frozenlake_vis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asschude/Documents/PhD/code/bprl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D27A37-15E6-144A-9753-D44B8425D5D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD5D438-955A-B748-BA2A-C9023A906181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="24660" windowHeight="14980" activeTab="1" xr2:uid="{B25F9FEF-11B1-CB41-8C01-2BCF7CAA3E3D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>[0, 0, 0, 0]</t>
   </si>
@@ -67,37 +67,37 @@
     <t>H</t>
   </si>
   <si>
-    <t>[0.5467946913319073, 0.47434364282157493, 0.40688994223825536, 0.4112479863533923]</t>
-  </si>
-  <si>
-    <t>[0.2801473017625735, 0.06080978418977151, 0.15582806760456647, 0.36613842079790687]</t>
-  </si>
-  <si>
-    <t>[0.3014242449992514, 0.1991887358739341, 0.19121089112800058, 0.20597158066709237]</t>
-  </si>
-  <si>
-    <t>[0.06909342152858103, 0.004611406193908754, 0.011775691072123923, 0.014097445057567435]</t>
-  </si>
-  <si>
-    <t>[0.5707396767397364, 0.40641768503661907, 0.2234778116040812, 0.3449412398743622]</t>
-  </si>
-  <si>
-    <t>[0.2105168396250403, 0.07348519915445617, 0.08089844294824658, 0.0]</t>
-  </si>
-  <si>
-    <t>[0.4029115989666619, 0.2842581443592238, 0.24282992851995813, 0.6190946425198655]</t>
-  </si>
-  <si>
-    <t>[0.32563940575461464, 0.586277912259295, 0.15364850521517434, 0.2405763965195443]</t>
-  </si>
-  <si>
-    <t>[0.6371268525657331, 0.2734002438609734, 0.3512311953981431, 0.22122113372727428]</t>
-  </si>
-  <si>
-    <t>[0.5410027964784536, 0.30781701757214774, 0.8085629239928983, 0.4111714499394089]</t>
-  </si>
-  <si>
-    <t>[0.6441281300785989, 0.9576927391751994, 0.6809332596653654, 0.651903587358928]</t>
+    <t>[0.1180411791224049, 0.13132008431689968, 0.3006348332760258, 0.11742772809842858]</t>
+  </si>
+  <si>
+    <t>[0.08155202445792062, 0.09276237251596907, 0.052045774211913656, 0.2932160519932141]</t>
+  </si>
+  <si>
+    <t>[0.3008774685687964, 0.08752969731758792, 0.08124246946025976, 0.07296432057025733]</t>
+  </si>
+  <si>
+    <t>[0.061906520871883676, 0.012155490812034951, 0.0, 0.0]</t>
+  </si>
+  <si>
+    <t>[0.3228427171213663, 0.030820952937119384, 0.06525290427062351, 0.029360025603771312]</t>
+  </si>
+  <si>
+    <t>[0.05013799414714607, 0.048124643114454975, 0.26202681968465635, 0.02931566738311541]</t>
+  </si>
+  <si>
+    <t>[0.06033929165086714, 0.014874866319464681, 0.11345250556429262, 0.39915711887421396]</t>
+  </si>
+  <si>
+    <t>[0.1769599218351724, 0.45921204987907416, 0.0, 0.06378724952988753]</t>
+  </si>
+  <si>
+    <t>[0.5881745366678465, 0.06407734442809308, 0.16684743801096957, 0.00899879364137959]</t>
+  </si>
+  <si>
+    <t>[0.0844034695101581, 0.1181536353695258, 0.5345872269876748, 0.1298342497318868]</t>
+  </si>
+  <si>
+    <t>[0.17556254791456682, 0.7441044850428351, 0.3640299822251991, 0.3638178538894259]</t>
   </si>
 </sst>
 </file>
@@ -119,12 +119,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -154,13 +160,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,31 +530,31 @@
       </c>
       <c r="J2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2,"[",""),"]",""),", ",";"),".",",")</f>
-        <v>0,5467946913319073;0,47434364282157493;0,40688994223825536;0,4112479863533923</v>
+        <v>0,1180411791224049;0,13132008431689968;0,3006348332760258;0,11742772809842858</v>
       </c>
       <c r="K2" t="str">
         <f>LEFT(J2,SEARCH(";",J2)-1)</f>
-        <v>0,5467946913319073</v>
+        <v>0,1180411791224049</v>
       </c>
       <c r="L2" t="str">
         <f>RIGHT(J2,LEN(J2)-SEARCH(";",J2))</f>
-        <v>0,47434364282157493;0,40688994223825536;0,4112479863533923</v>
+        <v>0,13132008431689968;0,3006348332760258;0,11742772809842858</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:R2" si="0">LEFT(L2,SEARCH(";",L2)-1)</f>
-        <v>0,47434364282157493</v>
+        <f t="shared" ref="M2" si="0">LEFT(L2,SEARCH(";",L2)-1)</f>
+        <v>0,13132008431689968</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" ref="N2" si="1">RIGHT(L2,LEN(L2)-SEARCH(";",L2))</f>
-        <v>0,40688994223825536;0,4112479863533923</v>
+        <v>0,3006348332760258;0,11742772809842858</v>
       </c>
       <c r="O2" t="str">
-        <f t="shared" ref="O2:R2" si="2">LEFT(N2,SEARCH(";",N2)-1)</f>
-        <v>0,40688994223825536</v>
+        <f t="shared" ref="O2" si="2">LEFT(N2,SEARCH(";",N2)-1)</f>
+        <v>0,3006348332760258</v>
       </c>
       <c r="P2" t="str">
         <f t="shared" ref="P2" si="3">RIGHT(N2,LEN(N2)-SEARCH(";",N2))</f>
-        <v>0,4112479863533923</v>
+        <v>0,11742772809842858</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -554,31 +563,31 @@
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J16" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3,"[",""),"]",""),", ",";"),".",",")</f>
-        <v>0,2801473017625735;0,06080978418977151;0,15582806760456647;0,36613842079790687</v>
+        <v>0,08155202445792062;0,09276237251596907;0,052045774211913656;0,2932160519932141</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K17" si="5">LEFT(J3,SEARCH(";",J3)-1)</f>
-        <v>0,2801473017625735</v>
+        <v>0,08155202445792062</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L16" si="6">RIGHT(J3,LEN(J3)-SEARCH(";",J3))</f>
-        <v>0,06080978418977151;0,15582806760456647;0,36613842079790687</v>
+        <v>0,09276237251596907;0,052045774211913656;0,2932160519932141</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:P3" si="7">LEFT(L3,SEARCH(";",L3)-1)</f>
-        <v>0,06080978418977151</v>
+        <f t="shared" ref="M3" si="7">LEFT(L3,SEARCH(";",L3)-1)</f>
+        <v>0,09276237251596907</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N16" si="8">RIGHT(L3,LEN(L3)-SEARCH(";",L3))</f>
-        <v>0,15582806760456647;0,36613842079790687</v>
+        <v>0,052045774211913656;0,2932160519932141</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:P3" si="9">LEFT(N3,SEARCH(";",N3)-1)</f>
-        <v>0,15582806760456647</v>
+        <f t="shared" ref="O3" si="9">LEFT(N3,SEARCH(";",N3)-1)</f>
+        <v>0,052045774211913656</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" ref="P3:P16" si="10">RIGHT(N3,LEN(N3)-SEARCH(";",N3))</f>
-        <v>0,36613842079790687</v>
+        <v>0,2932160519932141</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -587,31 +596,31 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="4"/>
-        <v>0,3014242449992514;0,1991887358739341;0,19121089112800058;0,20597158066709237</v>
+        <v>0,3008774685687964;0,08752969731758792;0,08124246946025976;0,07296432057025733</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="5"/>
-        <v>0,3014242449992514</v>
+        <v>0,3008774685687964</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="6"/>
-        <v>0,1991887358739341;0,19121089112800058;0,20597158066709237</v>
+        <v>0,08752969731758792;0,08124246946025976;0,07296432057025733</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:P4" si="11">LEFT(L4,SEARCH(";",L4)-1)</f>
-        <v>0,1991887358739341</v>
+        <f t="shared" ref="M4" si="11">LEFT(L4,SEARCH(";",L4)-1)</f>
+        <v>0,08752969731758792</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="8"/>
-        <v>0,19121089112800058;0,20597158066709237</v>
+        <v>0,08124246946025976;0,07296432057025733</v>
       </c>
       <c r="O4" t="str">
-        <f t="shared" ref="O4:P4" si="12">LEFT(N4,SEARCH(";",N4)-1)</f>
-        <v>0,19121089112800058</v>
+        <f t="shared" ref="O4" si="12">LEFT(N4,SEARCH(";",N4)-1)</f>
+        <v>0,08124246946025976</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" si="10"/>
-        <v>0,20597158066709237</v>
+        <v>0,07296432057025733</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -620,31 +629,31 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="4"/>
-        <v>0,06909342152858103;0,004611406193908754;0,011775691072123923;0,014097445057567435</v>
+        <v>0,061906520871883676;0,012155490812034951;0,0;0,0</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="5"/>
-        <v>0,06909342152858103</v>
+        <v>0,061906520871883676</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="6"/>
-        <v>0,004611406193908754;0,011775691072123923;0,014097445057567435</v>
+        <v>0,012155490812034951;0,0;0,0</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" ref="M5:P5" si="13">LEFT(L5,SEARCH(";",L5)-1)</f>
-        <v>0,004611406193908754</v>
+        <f t="shared" ref="M5" si="13">LEFT(L5,SEARCH(";",L5)-1)</f>
+        <v>0,012155490812034951</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="8"/>
-        <v>0,011775691072123923;0,014097445057567435</v>
+        <v>0,0;0,0</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:P5" si="14">LEFT(N5,SEARCH(";",N5)-1)</f>
-        <v>0,011775691072123923</v>
+        <f t="shared" ref="O5" si="14">LEFT(N5,SEARCH(";",N5)-1)</f>
+        <v>0,0</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="10"/>
-        <v>0,014097445057567435</v>
+        <v>0,0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -653,31 +662,31 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="4"/>
-        <v>0,5707396767397364;0,40641768503661907;0,2234778116040812;0,3449412398743622</v>
+        <v>0,3228427171213663;0,030820952937119384;0,06525290427062351;0,029360025603771312</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="5"/>
-        <v>0,5707396767397364</v>
+        <v>0,3228427171213663</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="6"/>
-        <v>0,40641768503661907;0,2234778116040812;0,3449412398743622</v>
+        <v>0,030820952937119384;0,06525290427062351;0,029360025603771312</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" ref="M6:P6" si="15">LEFT(L6,SEARCH(";",L6)-1)</f>
-        <v>0,40641768503661907</v>
+        <f t="shared" ref="M6" si="15">LEFT(L6,SEARCH(";",L6)-1)</f>
+        <v>0,030820952937119384</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="8"/>
-        <v>0,2234778116040812;0,3449412398743622</v>
+        <v>0,06525290427062351;0,029360025603771312</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" ref="O6:P6" si="16">LEFT(N6,SEARCH(";",N6)-1)</f>
-        <v>0,2234778116040812</v>
+        <f t="shared" ref="O6" si="16">LEFT(N6,SEARCH(";",N6)-1)</f>
+        <v>0,06525290427062351</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="10"/>
-        <v>0,3449412398743622</v>
+        <v>0,029360025603771312</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -697,7 +706,7 @@
         <v>0;0;0</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" ref="M7:P7" si="17">LEFT(L7,SEARCH(";",L7)-1)</f>
+        <f t="shared" ref="M7" si="17">LEFT(L7,SEARCH(";",L7)-1)</f>
         <v>0</v>
       </c>
       <c r="N7" t="str">
@@ -705,7 +714,7 @@
         <v>0;0</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" ref="O7:P7" si="18">LEFT(N7,SEARCH(";",N7)-1)</f>
+        <f t="shared" ref="O7" si="18">LEFT(N7,SEARCH(";",N7)-1)</f>
         <v>0</v>
       </c>
       <c r="P7" t="str">
@@ -719,31 +728,31 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="4"/>
-        <v>0,2105168396250403;0,07348519915445617;0,08089844294824658;0,0</v>
+        <v>0,05013799414714607;0,048124643114454975;0,26202681968465635;0,02931566738311541</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="5"/>
-        <v>0,2105168396250403</v>
+        <v>0,05013799414714607</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="6"/>
-        <v>0,07348519915445617;0,08089844294824658;0,0</v>
+        <v>0,048124643114454975;0,26202681968465635;0,02931566738311541</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" ref="M8:P8" si="19">LEFT(L8,SEARCH(";",L8)-1)</f>
-        <v>0,07348519915445617</v>
+        <f t="shared" ref="M8" si="19">LEFT(L8,SEARCH(";",L8)-1)</f>
+        <v>0,048124643114454975</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="8"/>
-        <v>0,08089844294824658;0,0</v>
+        <v>0,26202681968465635;0,02931566738311541</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ref="O8:P8" si="20">LEFT(N8,SEARCH(";",N8)-1)</f>
-        <v>0,08089844294824658</v>
+        <f t="shared" ref="O8" si="20">LEFT(N8,SEARCH(";",N8)-1)</f>
+        <v>0,26202681968465635</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="10"/>
-        <v>0,0</v>
+        <v>0,02931566738311541</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -763,7 +772,7 @@
         <v>0;0;0</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" ref="M9:P9" si="21">LEFT(L9,SEARCH(";",L9)-1)</f>
+        <f t="shared" ref="M9" si="21">LEFT(L9,SEARCH(";",L9)-1)</f>
         <v>0</v>
       </c>
       <c r="N9" t="str">
@@ -771,7 +780,7 @@
         <v>0;0</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" ref="O9:P9" si="22">LEFT(N9,SEARCH(";",N9)-1)</f>
+        <f t="shared" ref="O9" si="22">LEFT(N9,SEARCH(";",N9)-1)</f>
         <v>0</v>
       </c>
       <c r="P9" t="str">
@@ -785,31 +794,31 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="4"/>
-        <v>0,4029115989666619;0,2842581443592238;0,24282992851995813;0,6190946425198655</v>
+        <v>0,06033929165086714;0,014874866319464681;0,11345250556429262;0,39915711887421396</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="5"/>
-        <v>0,4029115989666619</v>
+        <v>0,06033929165086714</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="6"/>
-        <v>0,2842581443592238;0,24282992851995813;0,6190946425198655</v>
+        <v>0,014874866319464681;0,11345250556429262;0,39915711887421396</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" ref="M10:P10" si="23">LEFT(L10,SEARCH(";",L10)-1)</f>
-        <v>0,2842581443592238</v>
+        <f t="shared" ref="M10" si="23">LEFT(L10,SEARCH(";",L10)-1)</f>
+        <v>0,014874866319464681</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="8"/>
-        <v>0,24282992851995813;0,6190946425198655</v>
+        <v>0,11345250556429262;0,39915711887421396</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" ref="O10:P10" si="24">LEFT(N10,SEARCH(";",N10)-1)</f>
-        <v>0,24282992851995813</v>
+        <f t="shared" ref="O10" si="24">LEFT(N10,SEARCH(";",N10)-1)</f>
+        <v>0,11345250556429262</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="10"/>
-        <v>0,6190946425198655</v>
+        <v>0,39915711887421396</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -818,31 +827,31 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="4"/>
-        <v>0,32563940575461464;0,586277912259295;0,15364850521517434;0,2405763965195443</v>
+        <v>0,1769599218351724;0,45921204987907416;0,0;0,06378724952988753</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="5"/>
-        <v>0,32563940575461464</v>
+        <v>0,1769599218351724</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="6"/>
-        <v>0,586277912259295;0,15364850521517434;0,2405763965195443</v>
+        <v>0,45921204987907416;0,0;0,06378724952988753</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" ref="M11:P11" si="25">LEFT(L11,SEARCH(";",L11)-1)</f>
-        <v>0,586277912259295</v>
+        <f t="shared" ref="M11" si="25">LEFT(L11,SEARCH(";",L11)-1)</f>
+        <v>0,45921204987907416</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="8"/>
-        <v>0,15364850521517434;0,2405763965195443</v>
+        <v>0,0;0,06378724952988753</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" ref="O11:P11" si="26">LEFT(N11,SEARCH(";",N11)-1)</f>
-        <v>0,15364850521517434</v>
+        <f t="shared" ref="O11" si="26">LEFT(N11,SEARCH(";",N11)-1)</f>
+        <v>0,0</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" si="10"/>
-        <v>0,2405763965195443</v>
+        <v>0,06378724952988753</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -851,31 +860,31 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="4"/>
-        <v>0,6371268525657331;0,2734002438609734;0,3512311953981431;0,22122113372727428</v>
+        <v>0,5881745366678465;0,06407734442809308;0,16684743801096957;0,00899879364137959</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="5"/>
-        <v>0,6371268525657331</v>
+        <v>0,5881745366678465</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="6"/>
-        <v>0,2734002438609734;0,3512311953981431;0,22122113372727428</v>
+        <v>0,06407734442809308;0,16684743801096957;0,00899879364137959</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" ref="M12:P12" si="27">LEFT(L12,SEARCH(";",L12)-1)</f>
-        <v>0,2734002438609734</v>
+        <f t="shared" ref="M12" si="27">LEFT(L12,SEARCH(";",L12)-1)</f>
+        <v>0,06407734442809308</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="8"/>
-        <v>0,3512311953981431;0,22122113372727428</v>
+        <v>0,16684743801096957;0,00899879364137959</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" ref="O12:P12" si="28">LEFT(N12,SEARCH(";",N12)-1)</f>
-        <v>0,3512311953981431</v>
+        <f t="shared" ref="O12" si="28">LEFT(N12,SEARCH(";",N12)-1)</f>
+        <v>0,16684743801096957</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="10"/>
-        <v>0,22122113372727428</v>
+        <v>0,00899879364137959</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -895,7 +904,7 @@
         <v>0;0;0</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" ref="M13:P13" si="29">LEFT(L13,SEARCH(";",L13)-1)</f>
+        <f t="shared" ref="M13" si="29">LEFT(L13,SEARCH(";",L13)-1)</f>
         <v>0</v>
       </c>
       <c r="N13" t="str">
@@ -903,7 +912,7 @@
         <v>0;0</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" ref="O13:P13" si="30">LEFT(N13,SEARCH(";",N13)-1)</f>
+        <f t="shared" ref="O13" si="30">LEFT(N13,SEARCH(";",N13)-1)</f>
         <v>0</v>
       </c>
       <c r="P13" t="str">
@@ -928,7 +937,7 @@
         <v>0;0;0</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" ref="M14:P14" si="31">LEFT(L14,SEARCH(";",L14)-1)</f>
+        <f t="shared" ref="M14" si="31">LEFT(L14,SEARCH(";",L14)-1)</f>
         <v>0</v>
       </c>
       <c r="N14" t="str">
@@ -936,7 +945,7 @@
         <v>0;0</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" ref="O14:P14" si="32">LEFT(N14,SEARCH(";",N14)-1)</f>
+        <f t="shared" ref="O14" si="32">LEFT(N14,SEARCH(";",N14)-1)</f>
         <v>0</v>
       </c>
       <c r="P14" t="str">
@@ -950,31 +959,31 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="4"/>
-        <v>0,5410027964784536;0,30781701757214774;0,8085629239928983;0,4111714499394089</v>
+        <v>0,0844034695101581;0,1181536353695258;0,5345872269876748;0,1298342497318868</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="5"/>
-        <v>0,5410027964784536</v>
+        <v>0,0844034695101581</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="6"/>
-        <v>0,30781701757214774;0,8085629239928983;0,4111714499394089</v>
+        <v>0,1181536353695258;0,5345872269876748;0,1298342497318868</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" ref="M15:P15" si="33">LEFT(L15,SEARCH(";",L15)-1)</f>
-        <v>0,30781701757214774</v>
+        <f t="shared" ref="M15" si="33">LEFT(L15,SEARCH(";",L15)-1)</f>
+        <v>0,1181536353695258</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="8"/>
-        <v>0,8085629239928983;0,4111714499394089</v>
+        <v>0,5345872269876748;0,1298342497318868</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" ref="O15:P15" si="34">LEFT(N15,SEARCH(";",N15)-1)</f>
-        <v>0,8085629239928983</v>
+        <f t="shared" ref="O15" si="34">LEFT(N15,SEARCH(";",N15)-1)</f>
+        <v>0,5345872269876748</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="10"/>
-        <v>0,4111714499394089</v>
+        <v>0,1298342497318868</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -983,31 +992,31 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="4"/>
-        <v>0,6441281300785989;0,9576927391751994;0,6809332596653654;0,651903587358928</v>
+        <v>0,17556254791456682;0,7441044850428351;0,3640299822251991;0,3638178538894259</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="5"/>
-        <v>0,6441281300785989</v>
+        <v>0,17556254791456682</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="6"/>
-        <v>0,9576927391751994;0,6809332596653654;0,651903587358928</v>
+        <v>0,7441044850428351;0,3640299822251991;0,3638178538894259</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" ref="M16:P17" si="35">LEFT(L16,SEARCH(";",L16)-1)</f>
-        <v>0,9576927391751994</v>
+        <f t="shared" ref="M16:M17" si="35">LEFT(L16,SEARCH(";",L16)-1)</f>
+        <v>0,7441044850428351</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="8"/>
-        <v>0,6809332596653654;0,651903587358928</v>
+        <v>0,3640299822251991;0,3638178538894259</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" ref="O16:P17" si="36">LEFT(N16,SEARCH(";",N16)-1)</f>
-        <v>0,6809332596653654</v>
+        <f t="shared" ref="O16:O17" si="36">LEFT(N16,SEARCH(";",N16)-1)</f>
+        <v>0,3640299822251991</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="10"/>
-        <v>0,651903587358928</v>
+        <v>0,3638178538894259</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -1053,7 +1062,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,19 +1116,19 @@
       </c>
       <c r="B2" s="1">
         <f>VALUE(paste_here!K2)</f>
-        <v>0.54679469133190695</v>
+        <v>0.118041179122404</v>
       </c>
       <c r="C2">
         <f>VALUE(paste_here!M2)</f>
-        <v>0.47434364282157399</v>
+        <v>0.13132008431689901</v>
       </c>
       <c r="D2">
         <f>VALUE(paste_here!O2)</f>
-        <v>0.40688994223825498</v>
+        <v>0.30063483327602503</v>
       </c>
       <c r="E2">
         <f>VALUE(paste_here!P2)</f>
-        <v>0.41124798635339199</v>
+        <v>0.117427728098428</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
@@ -1127,25 +1136,25 @@
       </c>
       <c r="I2" s="2">
         <f>INDEX($B$2:$E$17,$G3*4+I$1+1,4)</f>
-        <v>0.41124798635339199</v>
+        <v>0.117427728098428</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2">
         <f t="shared" ref="L2" si="0">INDEX($B$2:$E$17,$G3*4+L$1+1,4)</f>
-        <v>0.36613842079790598</v>
+        <v>0.29321605199321399</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2">
         <f t="shared" ref="O2" si="1">INDEX($B$2:$E$17,$G3*4+O$1+1,4)</f>
-        <v>0.20597158066709201</v>
+        <v>7.2964320570257299E-2</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2">
         <f t="shared" ref="R2" si="2">INDEX($B$2:$E$17,$G3*4+R$1+1,4)</f>
-        <v>1.4097445057567401E-2</v>
+        <v>0</v>
       </c>
       <c r="S2" s="2"/>
     </row>
@@ -1156,70 +1165,70 @@
       </c>
       <c r="B3" s="1">
         <f>VALUE(paste_here!K3)</f>
-        <v>0.28014730176257302</v>
+        <v>8.1552024457920605E-2</v>
       </c>
       <c r="C3">
         <f>VALUE(paste_here!M3)</f>
-        <v>6.0809784189771503E-2</v>
+        <v>9.2762372515968999E-2</v>
       </c>
       <c r="D3">
         <f>VALUE(paste_here!O3)</f>
-        <v>0.155828067604566</v>
+        <v>5.2045774211913601E-2</v>
       </c>
       <c r="E3">
         <f>VALUE(paste_here!P3)</f>
-        <v>0.36613842079790598</v>
+        <v>0.29321605199321399</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="2">
         <f>INDEX($B$2:$E$17,$G3*4+I$1+1,1)</f>
-        <v>0.54679469133190695</v>
+        <v>0.118041179122404</v>
       </c>
       <c r="I3" s="3">
         <f>AVERAGE(I2,H3,I4,J3)</f>
-        <v>0.459819065686282</v>
+        <v>0.16685595620343902</v>
       </c>
       <c r="J3" s="2">
         <f>INDEX($B$2:$E$17,$G3*4+I$1+1,3)</f>
-        <v>0.40688994223825498</v>
+        <v>0.30063483327602503</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:S3" si="3">INDEX($B$2:$E$17,$G3*4+L$1+1,1)</f>
-        <v>0.28014730176257302</v>
+        <f t="shared" ref="K3" si="3">INDEX($B$2:$E$17,$G3*4+L$1+1,1)</f>
+        <v>8.1552024457920605E-2</v>
       </c>
       <c r="L3" s="3">
         <f t="shared" ref="L3" si="4">AVERAGE(L2,K3,L4,M3)</f>
-        <v>0.21573089358870412</v>
+        <v>0.1298940557947543</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:S3" si="5">INDEX($B$2:$E$17,$G3*4+L$1+1,3)</f>
-        <v>0.155828067604566</v>
+        <f t="shared" ref="M3" si="5">INDEX($B$2:$E$17,$G3*4+L$1+1,3)</f>
+        <v>5.2045774211913601E-2</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" ref="N3:S3" si="6">INDEX($B$2:$E$17,$G3*4+O$1+1,1)</f>
-        <v>0.30142424499925102</v>
+        <f t="shared" ref="N3" si="6">INDEX($B$2:$E$17,$G3*4+O$1+1,1)</f>
+        <v>0.30087746856879599</v>
       </c>
       <c r="O3" s="3">
         <f t="shared" ref="O3" si="7">AVERAGE(O2,N3,O4,P3)</f>
-        <v>0.22444886316706925</v>
+        <v>0.13565348897922525</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" ref="P3:S3" si="8">INDEX($B$2:$E$17,$G3*4+O$1+1,3)</f>
-        <v>0.19121089112799999</v>
+        <f t="shared" ref="P3" si="8">INDEX($B$2:$E$17,$G3*4+O$1+1,3)</f>
+        <v>8.1242469460259703E-2</v>
       </c>
       <c r="Q3" s="2">
-        <f t="shared" ref="Q3:S3" si="9">INDEX($B$2:$E$17,$G3*4+R$1+1,1)</f>
-        <v>6.9093421528581001E-2</v>
+        <f t="shared" ref="Q3" si="9">INDEX($B$2:$E$17,$G3*4+R$1+1,1)</f>
+        <v>6.19065208718836E-2</v>
       </c>
       <c r="R3" s="3">
         <f t="shared" ref="R3" si="10">AVERAGE(R2,Q3,R4,S3)</f>
-        <v>2.489449096304526E-2</v>
+        <v>1.8515502920979626E-2</v>
       </c>
       <c r="S3" s="2">
         <f t="shared" ref="S3" si="11">INDEX($B$2:$E$17,$G3*4+R$1+1,3)</f>
-        <v>1.17756910721239E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1229,43 +1238,43 @@
       </c>
       <c r="B4" s="1">
         <f>VALUE(paste_here!K4)</f>
-        <v>0.30142424499925102</v>
+        <v>0.30087746856879599</v>
       </c>
       <c r="C4">
         <f>VALUE(paste_here!M4)</f>
-        <v>0.19918873587393399</v>
+        <v>8.7529697317587904E-2</v>
       </c>
       <c r="D4">
         <f>VALUE(paste_here!O4)</f>
-        <v>0.19121089112799999</v>
+        <v>8.1242469460259703E-2</v>
       </c>
       <c r="E4">
         <f>VALUE(paste_here!P4)</f>
-        <v>0.20597158066709201</v>
+        <v>7.2964320570257299E-2</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2">
         <f>INDEX($B$2:$E$17,$G3*4+I$1+1,2)</f>
-        <v>0.47434364282157399</v>
+        <v>0.13132008431689901</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2">
         <f t="shared" ref="L4" si="13">INDEX($B$2:$E$17,$G3*4+L$1+1,2)</f>
-        <v>6.0809784189771503E-2</v>
+        <v>9.2762372515968999E-2</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2">
         <f t="shared" ref="O4" si="14">INDEX($B$2:$E$17,$G3*4+O$1+1,2)</f>
-        <v>0.19918873587393399</v>
+        <v>8.7529697317587904E-2</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2">
         <f t="shared" ref="R4" si="15">INDEX($B$2:$E$17,$G3*4+R$1+1,2)</f>
-        <v>4.6114061939087504E-3</v>
+        <v>1.2155490812034901E-2</v>
       </c>
       <c r="S4" s="2"/>
     </row>
@@ -1276,46 +1285,42 @@
       </c>
       <c r="B5" s="1">
         <f>VALUE(paste_here!K5)</f>
-        <v>6.9093421528581001E-2</v>
+        <v>6.19065208718836E-2</v>
       </c>
       <c r="C5">
         <f>VALUE(paste_here!M5)</f>
-        <v>4.6114061939087504E-3</v>
+        <v>1.2155490812034901E-2</v>
       </c>
       <c r="D5">
         <f>VALUE(paste_here!O5)</f>
-        <v>1.17756910721239E-2</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f>VALUE(paste_here!P5)</f>
-        <v>1.4097445057567401E-2</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I13" si="16">INDEX($B$2:$E$17,$G6*4+I$1+1,4)</f>
-        <v>0.34494123987436198</v>
+        <f t="shared" ref="I5" si="16">INDEX($B$2:$E$17,$G6*4+I$1+1,4)</f>
+        <v>2.9360025603771302E-2</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="K5" s="2"/>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L13" si="17">INDEX($B$2:$E$17,$G6*4+L$1+1,4)</f>
+        <f t="shared" ref="L5" si="17">INDEX($B$2:$E$17,$G6*4+L$1+1,4)</f>
         <v>0</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2">
-        <f t="shared" ref="O5:O13" si="18">INDEX($B$2:$E$17,$G6*4+O$1+1,4)</f>
-        <v>0</v>
+        <f t="shared" ref="O5" si="18">INDEX($B$2:$E$17,$G6*4+O$1+1,4)</f>
+        <v>2.9315667383115401E-2</v>
       </c>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="Q5" s="2"/>
       <c r="R5" s="2">
-        <f t="shared" ref="R5:R13" si="19">INDEX($B$2:$E$17,$G6*4+R$1+1,4)</f>
+        <f t="shared" ref="R5" si="19">INDEX($B$2:$E$17,$G6*4+R$1+1,4)</f>
         <v>0</v>
       </c>
       <c r="S5" s="2"/>
@@ -1327,64 +1332,64 @@
       </c>
       <c r="B6" s="1">
         <f>VALUE(paste_here!K6)</f>
-        <v>0.57073967673973602</v>
+        <v>0.32284271712136597</v>
       </c>
       <c r="C6">
         <f>VALUE(paste_here!M6)</f>
-        <v>0.40641768503661901</v>
+        <v>3.0820952937119301E-2</v>
       </c>
       <c r="D6">
         <f>VALUE(paste_here!O6)</f>
-        <v>0.22347781160408101</v>
+        <v>6.5252904270623496E-2</v>
       </c>
       <c r="E6">
         <f>VALUE(paste_here!P6)</f>
-        <v>0.34494123987436198</v>
+        <v>2.9360025603771302E-2</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ref="H6" si="20">INDEX($B$2:$E$17,$G6*4+I$1+1,1)</f>
-        <v>0.57073967673973602</v>
+        <v>0.32284271712136597</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" ref="I6" si="21">AVERAGE(I5,H6,I7,J6)</f>
-        <v>0.3863941033136995</v>
+        <v>0.11206914998322001</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ref="J6" si="22">INDEX($B$2:$E$17,$G6*4+I$1+1,3)</f>
-        <v>0.22347781160408101</v>
+        <v>6.5252904270623496E-2</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:S6" si="23">INDEX($B$2:$E$17,$G6*4+L$1+1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
+        <f t="shared" ref="K6" si="23">INDEX($B$2:$E$17,$G6*4+L$1+1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <f t="shared" ref="L6" si="24">AVERAGE(L5,K6,L7,M6)</f>
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" ref="M6:S6" si="25">INDEX($B$2:$E$17,$G6*4+L$1+1,3)</f>
+        <f t="shared" ref="M6" si="25">INDEX($B$2:$E$17,$G6*4+L$1+1,3)</f>
         <v>0</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" ref="N6:S6" si="26">INDEX($B$2:$E$17,$G6*4+O$1+1,1)</f>
-        <v>0.21051683962504</v>
+        <f t="shared" ref="N6" si="26">INDEX($B$2:$E$17,$G6*4+O$1+1,1)</f>
+        <v>5.0137994147146002E-2</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" ref="O6" si="27">AVERAGE(O5,N6,O7,P6)</f>
-        <v>9.1225120431935647E-2</v>
+        <v>9.7401281082343083E-2</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" ref="P6:S6" si="28">INDEX($B$2:$E$17,$G6*4+O$1+1,3)</f>
-        <v>8.0898442948246496E-2</v>
+        <f t="shared" ref="P6" si="28">INDEX($B$2:$E$17,$G6*4+O$1+1,3)</f>
+        <v>0.26202681968465602</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" ref="Q6:S6" si="29">INDEX($B$2:$E$17,$G6*4+R$1+1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
+        <f t="shared" ref="Q6" si="29">INDEX($B$2:$E$17,$G6*4+R$1+1,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
         <f t="shared" ref="R6" si="30">AVERAGE(R5,Q6,R7,S6)</f>
         <v>0</v>
       </c>
@@ -1417,25 +1422,25 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2">
-        <f t="shared" ref="I7:I13" si="32">INDEX($B$2:$E$17,$G6*4+I$1+1,2)</f>
-        <v>0.40641768503661901</v>
+        <f t="shared" ref="I7" si="32">INDEX($B$2:$E$17,$G6*4+I$1+1,2)</f>
+        <v>3.0820952937119301E-2</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2">
-        <f t="shared" ref="L7:L13" si="33">INDEX($B$2:$E$17,$G6*4+L$1+1,2)</f>
+        <f t="shared" ref="L7" si="33">INDEX($B$2:$E$17,$G6*4+L$1+1,2)</f>
         <v>0</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2">
-        <f t="shared" ref="O7:O13" si="34">INDEX($B$2:$E$17,$G6*4+O$1+1,2)</f>
-        <v>7.3485199154456102E-2</v>
+        <f t="shared" ref="O7" si="34">INDEX($B$2:$E$17,$G6*4+O$1+1,2)</f>
+        <v>4.8124643114454899E-2</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2">
-        <f t="shared" ref="R7:R13" si="35">INDEX($B$2:$E$17,$G6*4+R$1+1,2)</f>
+        <f t="shared" ref="R7" si="35">INDEX($B$2:$E$17,$G6*4+R$1+1,2)</f>
         <v>0</v>
       </c>
       <c r="S7" s="2"/>
@@ -1447,44 +1452,44 @@
       </c>
       <c r="B8" s="1">
         <f>VALUE(paste_here!K8)</f>
-        <v>0.21051683962504</v>
+        <v>5.0137994147146002E-2</v>
       </c>
       <c r="C8">
         <f>VALUE(paste_here!M8)</f>
-        <v>7.3485199154456102E-2</v>
+        <v>4.8124643114454899E-2</v>
       </c>
       <c r="D8">
         <f>VALUE(paste_here!O8)</f>
-        <v>8.0898442948246496E-2</v>
+        <v>0.26202681968465602</v>
       </c>
       <c r="E8">
         <f>VALUE(paste_here!P8)</f>
-        <v>0</v>
+        <v>2.9315667383115401E-2</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2">
-        <f t="shared" ref="I8:I13" si="36">INDEX($B$2:$E$17,$G9*4+I$1+1,4)</f>
-        <v>0.61909464251986501</v>
+        <f t="shared" ref="I8" si="36">INDEX($B$2:$E$17,$G9*4+I$1+1,4)</f>
+        <v>0.39915711887421301</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2">
-        <f t="shared" ref="L8:L13" si="37">INDEX($B$2:$E$17,$G9*4+L$1+1,4)</f>
-        <v>0.24057639651954399</v>
+        <f t="shared" ref="L8" si="37">INDEX($B$2:$E$17,$G9*4+L$1+1,4)</f>
+        <v>6.3787249529887499E-2</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2">
-        <f t="shared" ref="O8:O13" si="38">INDEX($B$2:$E$17,$G9*4+O$1+1,4)</f>
-        <v>0.22122113372727401</v>
+        <f t="shared" ref="O8" si="38">INDEX($B$2:$E$17,$G9*4+O$1+1,4)</f>
+        <v>8.9987936413795898E-3</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R8" s="2">
-        <f t="shared" ref="R8:R13" si="39">INDEX($B$2:$E$17,$G9*4+R$1+1,4)</f>
+        <f t="shared" ref="R8" si="39">INDEX($B$2:$E$17,$G9*4+R$1+1,4)</f>
         <v>0</v>
       </c>
       <c r="S8" s="2"/>
@@ -1515,42 +1520,42 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" ref="H9" si="40">INDEX($B$2:$E$17,$G9*4+I$1+1,1)</f>
-        <v>0.40291159896666101</v>
+        <v>6.03392916508671E-2</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" ref="I9" si="41">AVERAGE(I8,H9,I10,J9)</f>
-        <v>0.38727357859142675</v>
+        <v>0.14695594560220918</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ref="J9" si="42">INDEX($B$2:$E$17,$G9*4+I$1+1,3)</f>
-        <v>0.24282992851995799</v>
+        <v>0.113452505564292</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" ref="K9:S9" si="43">INDEX($B$2:$E$17,$G9*4+L$1+1,1)</f>
-        <v>0.32563940575461398</v>
+        <f t="shared" ref="K9" si="43">INDEX($B$2:$E$17,$G9*4+L$1+1,1)</f>
+        <v>0.17695992183517201</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" ref="L9" si="44">AVERAGE(L8,K9,L10,M9)</f>
-        <v>0.32653555493715675</v>
+        <v>0.17498980531103336</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ref="M9:S9" si="45">INDEX($B$2:$E$17,$G9*4+L$1+1,3)</f>
-        <v>0.15364850521517401</v>
+        <f t="shared" ref="M9" si="45">INDEX($B$2:$E$17,$G9*4+L$1+1,3)</f>
+        <v>0</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" ref="N9:S9" si="46">INDEX($B$2:$E$17,$G9*4+O$1+1,1)</f>
-        <v>0.63712685256573298</v>
+        <f t="shared" ref="N9" si="46">INDEX($B$2:$E$17,$G9*4+O$1+1,1)</f>
+        <v>0.58817453666784603</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" ref="O9" si="47">AVERAGE(O8,N9,O10,P9)</f>
-        <v>0.37074485638803079</v>
+        <v>0.2070245281870719</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ref="P9:S9" si="48">INDEX($B$2:$E$17,$G9*4+O$1+1,3)</f>
-        <v>0.35123119539814301</v>
+        <f t="shared" ref="P9" si="48">INDEX($B$2:$E$17,$G9*4+O$1+1,3)</f>
+        <v>0.16684743801096899</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" ref="Q9:S9" si="49">INDEX($B$2:$E$17,$G9*4+R$1+1,1)</f>
+        <f t="shared" ref="Q9" si="49">INDEX($B$2:$E$17,$G9*4+R$1+1,1)</f>
         <v>0</v>
       </c>
       <c r="R9" s="3">
@@ -1569,42 +1574,42 @@
       </c>
       <c r="B10" s="1">
         <f>VALUE(paste_here!K10)</f>
-        <v>0.40291159896666101</v>
+        <v>6.03392916508671E-2</v>
       </c>
       <c r="C10">
         <f>VALUE(paste_here!M10)</f>
-        <v>0.28425814435922298</v>
+        <v>1.4874866319464599E-2</v>
       </c>
       <c r="D10">
         <f>VALUE(paste_here!O10)</f>
-        <v>0.24282992851995799</v>
+        <v>0.113452505564292</v>
       </c>
       <c r="E10">
         <f>VALUE(paste_here!P10)</f>
-        <v>0.61909464251986501</v>
+        <v>0.39915711887421301</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
-        <f t="shared" ref="I10:I13" si="51">INDEX($B$2:$E$17,$G9*4+I$1+1,2)</f>
-        <v>0.28425814435922298</v>
+        <f t="shared" ref="I10" si="51">INDEX($B$2:$E$17,$G9*4+I$1+1,2)</f>
+        <v>1.4874866319464599E-2</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2">
-        <f t="shared" ref="L10:L13" si="52">INDEX($B$2:$E$17,$G9*4+L$1+1,2)</f>
-        <v>0.58627791225929504</v>
+        <f t="shared" ref="L10" si="52">INDEX($B$2:$E$17,$G9*4+L$1+1,2)</f>
+        <v>0.45921204987907399</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2">
-        <f t="shared" ref="O10:O13" si="53">INDEX($B$2:$E$17,$G9*4+O$1+1,2)</f>
-        <v>0.273400243860973</v>
+        <f t="shared" ref="O10" si="53">INDEX($B$2:$E$17,$G9*4+O$1+1,2)</f>
+        <v>6.4077344428093E-2</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2">
-        <f t="shared" ref="R10:R13" si="54">INDEX($B$2:$E$17,$G9*4+R$1+1,2)</f>
+        <f t="shared" ref="R10" si="54">INDEX($B$2:$E$17,$G9*4+R$1+1,2)</f>
         <v>0</v>
       </c>
       <c r="S10" s="2"/>
@@ -1616,46 +1621,42 @@
       </c>
       <c r="B11" s="1">
         <f>VALUE(paste_here!K11)</f>
-        <v>0.32563940575461398</v>
+        <v>0.17695992183517201</v>
       </c>
       <c r="C11">
         <f>VALUE(paste_here!M11)</f>
-        <v>0.58627791225929504</v>
+        <v>0.45921204987907399</v>
       </c>
       <c r="D11">
         <f>VALUE(paste_here!O11)</f>
-        <v>0.15364850521517401</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <f>VALUE(paste_here!P11)</f>
-        <v>0.24057639651954399</v>
+        <v>6.3787249529887499E-2</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2">
-        <f t="shared" ref="I11:I13" si="55">INDEX($B$2:$E$17,$G12*4+I$1+1,4)</f>
+        <f t="shared" ref="I11" si="55">INDEX($B$2:$E$17,$G12*4+I$1+1,4)</f>
         <v>0</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2">
-        <f t="shared" ref="L11:L13" si="56">INDEX($B$2:$E$17,$G12*4+L$1+1,4)</f>
-        <v>0.41117144993940802</v>
+        <f t="shared" ref="L11" si="56">INDEX($B$2:$E$17,$G12*4+L$1+1,4)</f>
+        <v>0.12983424973188601</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2">
-        <f t="shared" ref="O11:O13" si="57">INDEX($B$2:$E$17,$G12*4+O$1+1,4)</f>
-        <v>0.65190358735892795</v>
+        <f t="shared" ref="O11" si="57">INDEX($B$2:$E$17,$G12*4+O$1+1,4)</f>
+        <v>0.363817853889425</v>
       </c>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="Q11" s="2"/>
       <c r="R11" s="2">
-        <f t="shared" ref="R11:R13" si="58">INDEX($B$2:$E$17,$G12*4+R$1+1,4)</f>
+        <f t="shared" ref="R11" si="58">INDEX($B$2:$E$17,$G12*4+R$1+1,4)</f>
         <v>0</v>
       </c>
       <c r="S11" s="2"/>
@@ -1667,19 +1668,19 @@
       </c>
       <c r="B12" s="1">
         <f>VALUE(paste_here!K12)</f>
-        <v>0.63712685256573298</v>
+        <v>0.58817453666784603</v>
       </c>
       <c r="C12">
         <f>VALUE(paste_here!M12)</f>
-        <v>0.273400243860973</v>
+        <v>6.4077344428093E-2</v>
       </c>
       <c r="D12">
         <f>VALUE(paste_here!O12)</f>
-        <v>0.35123119539814301</v>
+        <v>0.16684743801096899</v>
       </c>
       <c r="E12">
         <f>VALUE(paste_here!P12)</f>
-        <v>0.22122113372727401</v>
+        <v>8.9987936413795898E-3</v>
       </c>
       <c r="G12" s="2">
         <v>3</v>
@@ -1688,7 +1689,7 @@
         <f t="shared" ref="H12" si="59">INDEX($B$2:$E$17,$G12*4+I$1+1,1)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="4">
         <f t="shared" ref="I12" si="60">AVERAGE(I11,H12,I13,J12)</f>
         <v>0</v>
       </c>
@@ -1697,31 +1698,31 @@
         <v>0</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" ref="K12:S12" si="62">INDEX($B$2:$E$17,$G12*4+L$1+1,1)</f>
-        <v>0.54100279647845295</v>
+        <f t="shared" ref="K12" si="62">INDEX($B$2:$E$17,$G12*4+L$1+1,1)</f>
+        <v>8.4403469510158105E-2</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" ref="L12" si="63">AVERAGE(L11,K12,L13,M12)</f>
-        <v>0.51713854699572648</v>
+        <v>0.21674464539981078</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" ref="M12:S12" si="64">INDEX($B$2:$E$17,$G12*4+L$1+1,3)</f>
-        <v>0.80856292399289798</v>
+        <f t="shared" ref="M12" si="64">INDEX($B$2:$E$17,$G12*4+L$1+1,3)</f>
+        <v>0.53458722698767402</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" ref="N12:S12" si="65">INDEX($B$2:$E$17,$G12*4+O$1+1,1)</f>
-        <v>0.64412813007859804</v>
+        <f t="shared" ref="N12" si="65">INDEX($B$2:$E$17,$G12*4+O$1+1,1)</f>
+        <v>0.17556254791456599</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" ref="O12" si="66">AVERAGE(O11,N12,O13,P12)</f>
-        <v>0.73366442906952245</v>
+        <v>0.41187871726800618</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" ref="P12:S12" si="67">INDEX($B$2:$E$17,$G12*4+O$1+1,3)</f>
-        <v>0.680933259665365</v>
+        <f t="shared" ref="P12" si="67">INDEX($B$2:$E$17,$G12*4+O$1+1,3)</f>
+        <v>0.364029982225199</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" ref="Q12:S12" si="68">INDEX($B$2:$E$17,$G12*4+R$1+1,1)</f>
+        <f t="shared" ref="Q12" si="68">INDEX($B$2:$E$17,$G12*4+R$1+1,1)</f>
         <v>0</v>
       </c>
       <c r="R12" s="3">
@@ -1764,13 +1765,13 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2">
         <f t="shared" ref="L13" si="71">INDEX($B$2:$E$17,$G12*4+L$1+1,2)</f>
-        <v>0.30781701757214702</v>
+        <v>0.118153635369525</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2">
         <f t="shared" ref="O13" si="72">INDEX($B$2:$E$17,$G12*4+O$1+1,2)</f>
-        <v>0.95769273917519904</v>
+        <v>0.744104485042835</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1778,7 +1779,9 @@
         <f t="shared" ref="R13" si="73">INDEX($B$2:$E$17,$G12*4+R$1+1,2)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="2"/>
+      <c r="S13" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1809,19 +1812,19 @@
       </c>
       <c r="B15" s="1">
         <f>VALUE(paste_here!K15)</f>
-        <v>0.54100279647845295</v>
+        <v>8.4403469510158105E-2</v>
       </c>
       <c r="C15">
         <f>VALUE(paste_here!M15)</f>
-        <v>0.30781701757214702</v>
+        <v>0.118153635369525</v>
       </c>
       <c r="D15">
         <f>VALUE(paste_here!O15)</f>
-        <v>0.80856292399289798</v>
+        <v>0.53458722698767402</v>
       </c>
       <c r="E15">
         <f>VALUE(paste_here!P15)</f>
-        <v>0.41117144993940802</v>
+        <v>0.12983424973188601</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1831,19 +1834,19 @@
       </c>
       <c r="B16" s="1">
         <f>VALUE(paste_here!K16)</f>
-        <v>0.64412813007859804</v>
+        <v>0.17556254791456599</v>
       </c>
       <c r="C16">
         <f>VALUE(paste_here!M16)</f>
-        <v>0.95769273917519904</v>
+        <v>0.744104485042835</v>
       </c>
       <c r="D16">
         <f>VALUE(paste_here!O16)</f>
-        <v>0.680933259665365</v>
+        <v>0.364029982225199</v>
       </c>
       <c r="E16">
         <f>VALUE(paste_here!P16)</f>
-        <v>0.65190358735892795</v>
+        <v>0.363817853889425</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feature: fixed chart (font) sizes, visualized classic examples
</commit_message>
<xml_diff>
--- a/frozenlake_vis.xlsx
+++ b/frozenlake_vis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asschude/Documents/PhD/code/bprl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD5D438-955A-B748-BA2A-C9023A906181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CCE023-CBDB-3E47-B5DD-C0366B5D24C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="24660" windowHeight="14980" activeTab="1" xr2:uid="{B25F9FEF-11B1-CB41-8C01-2BCF7CAA3E3D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>[0, 0, 0, 0]</t>
   </si>
@@ -58,15 +58,6 @@
     <t>rest1</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>[0.1180411791224049, 0.13132008431689968, 0.3006348332760258, 0.11742772809842858]</t>
   </si>
   <si>
@@ -98,6 +89,12 @@
   </si>
   <si>
     <t>[0.17556254791456682, 0.7441044850428351, 0.3640299822251991, 0.3638178538894259]</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -119,7 +116,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,9 +124,15 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="lightUp">
         <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor auto="1"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,18 +163,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -526,7 +536,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A2,"[",""),"]",""),", ",";"),".",",")</f>
@@ -559,7 +569,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J16" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A3,"[",""),"]",""),", ",";"),".",",")</f>
@@ -592,7 +602,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="4"/>
@@ -625,7 +635,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="4"/>
@@ -658,7 +668,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="4"/>
@@ -724,7 +734,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="4"/>
@@ -790,7 +800,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="4"/>
@@ -823,7 +833,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="4"/>
@@ -856,7 +866,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="4"/>
@@ -955,7 +965,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="4"/>
@@ -988,7 +998,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="4"/>
@@ -1059,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8060249D-369B-A94F-B1C9-448D76A5E886}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1082,7 @@
     <col min="8" max="19" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1109,8 +1119,9 @@
         <v>3</v>
       </c>
       <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1131,8 +1142,8 @@
         <v>0.117427728098428</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="I2" s="2">
         <f>INDEX($B$2:$E$17,$G3*4+I$1+1,4)</f>
@@ -1157,8 +1168,9 @@
         <v>0</v>
       </c>
       <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" s="7"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1186,7 +1198,7 @@
         <f>INDEX($B$2:$E$17,$G3*4+I$1+1,1)</f>
         <v>0.118041179122404</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="4">
         <f>AVERAGE(I2,H3,I4,J3)</f>
         <v>0.16685595620343902</v>
       </c>
@@ -1198,7 +1210,7 @@
         <f t="shared" ref="K3" si="3">INDEX($B$2:$E$17,$G3*4+L$1+1,1)</f>
         <v>8.1552024457920605E-2</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="4">
         <f t="shared" ref="L3" si="4">AVERAGE(L2,K3,L4,M3)</f>
         <v>0.1298940557947543</v>
       </c>
@@ -1210,7 +1222,7 @@
         <f t="shared" ref="N3" si="6">INDEX($B$2:$E$17,$G3*4+O$1+1,1)</f>
         <v>0.30087746856879599</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="4">
         <f t="shared" ref="O3" si="7">AVERAGE(O2,N3,O4,P3)</f>
         <v>0.13565348897922525</v>
       </c>
@@ -1222,7 +1234,7 @@
         <f t="shared" ref="Q3" si="9">INDEX($B$2:$E$17,$G3*4+R$1+1,1)</f>
         <v>6.19065208718836E-2</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="4">
         <f t="shared" ref="R3" si="10">AVERAGE(R2,Q3,R4,S3)</f>
         <v>1.8515502920979626E-2</v>
       </c>
@@ -1230,8 +1242,9 @@
         <f t="shared" ref="S3" si="11">INDEX($B$2:$E$17,$G3*4+R$1+1,3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A17" si="12">A3+1</f>
         <v>3</v>
@@ -1277,8 +1290,9 @@
         <v>1.2155490812034901E-2</v>
       </c>
       <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="12"/>
         <v>4</v>
@@ -1324,8 +1338,9 @@
         <v>0</v>
       </c>
       <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="12"/>
         <v>5</v>
@@ -1353,7 +1368,7 @@
         <f t="shared" ref="H6" si="20">INDEX($B$2:$E$17,$G6*4+I$1+1,1)</f>
         <v>0.32284271712136597</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="4">
         <f t="shared" ref="I6" si="21">AVERAGE(I5,H6,I7,J6)</f>
         <v>0.11206914998322001</v>
       </c>
@@ -1365,7 +1380,7 @@
         <f t="shared" ref="K6" si="23">INDEX($B$2:$E$17,$G6*4+L$1+1,1)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="5">
         <f t="shared" ref="L6" si="24">AVERAGE(L5,K6,L7,M6)</f>
         <v>0</v>
       </c>
@@ -1377,7 +1392,7 @@
         <f t="shared" ref="N6" si="26">INDEX($B$2:$E$17,$G6*4+O$1+1,1)</f>
         <v>5.0137994147146002E-2</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="4">
         <f t="shared" ref="O6" si="27">AVERAGE(O5,N6,O7,P6)</f>
         <v>9.7401281082343083E-2</v>
       </c>
@@ -1389,7 +1404,7 @@
         <f t="shared" ref="Q6" si="29">INDEX($B$2:$E$17,$G6*4+R$1+1,1)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="5">
         <f t="shared" ref="R6" si="30">AVERAGE(R5,Q6,R7,S6)</f>
         <v>0</v>
       </c>
@@ -1397,8 +1412,9 @@
         <f t="shared" ref="S6:S12" si="31">INDEX($B$2:$E$17,$G6*4+R$1+1,3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="12"/>
         <v>6</v>
@@ -1444,8 +1460,9 @@
         <v>0</v>
       </c>
       <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="12"/>
         <v>7</v>
@@ -1485,16 +1502,15 @@
         <v>8.9987936413795898E-3</v>
       </c>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="Q8" s="2"/>
       <c r="R8" s="2">
         <f t="shared" ref="R8" si="39">INDEX($B$2:$E$17,$G9*4+R$1+1,4)</f>
         <v>0</v>
       </c>
       <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="12"/>
         <v>8</v>
@@ -1522,7 +1538,7 @@
         <f t="shared" ref="H9" si="40">INDEX($B$2:$E$17,$G9*4+I$1+1,1)</f>
         <v>6.03392916508671E-2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="4">
         <f t="shared" ref="I9" si="41">AVERAGE(I8,H9,I10,J9)</f>
         <v>0.14695594560220918</v>
       </c>
@@ -1534,7 +1550,7 @@
         <f t="shared" ref="K9" si="43">INDEX($B$2:$E$17,$G9*4+L$1+1,1)</f>
         <v>0.17695992183517201</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="4">
         <f t="shared" ref="L9" si="44">AVERAGE(L8,K9,L10,M9)</f>
         <v>0.17498980531103336</v>
       </c>
@@ -1546,7 +1562,7 @@
         <f t="shared" ref="N9" si="46">INDEX($B$2:$E$17,$G9*4+O$1+1,1)</f>
         <v>0.58817453666784603</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="4">
         <f t="shared" ref="O9" si="47">AVERAGE(O8,N9,O10,P9)</f>
         <v>0.2070245281870719</v>
       </c>
@@ -1558,7 +1574,7 @@
         <f t="shared" ref="Q9" si="49">INDEX($B$2:$E$17,$G9*4+R$1+1,1)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="5">
         <f t="shared" ref="R9" si="50">AVERAGE(R8,Q9,R10,S9)</f>
         <v>0</v>
       </c>
@@ -1566,8 +1582,9 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="12"/>
         <v>9</v>
@@ -1613,8 +1630,9 @@
         <v>0</v>
       </c>
       <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="12"/>
         <v>10</v>
@@ -1660,8 +1678,9 @@
         <v>0</v>
       </c>
       <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="12"/>
         <v>11</v>
@@ -1689,7 +1708,7 @@
         <f t="shared" ref="H12" si="59">INDEX($B$2:$E$17,$G12*4+I$1+1,1)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="5">
         <f t="shared" ref="I12" si="60">AVERAGE(I11,H12,I13,J12)</f>
         <v>0</v>
       </c>
@@ -1701,7 +1720,7 @@
         <f t="shared" ref="K12" si="62">INDEX($B$2:$E$17,$G12*4+L$1+1,1)</f>
         <v>8.4403469510158105E-2</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="4">
         <f t="shared" ref="L12" si="63">AVERAGE(L11,K12,L13,M12)</f>
         <v>0.21674464539981078</v>
       </c>
@@ -1713,7 +1732,7 @@
         <f t="shared" ref="N12" si="65">INDEX($B$2:$E$17,$G12*4+O$1+1,1)</f>
         <v>0.17556254791456599</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="4">
         <f t="shared" ref="O12" si="66">AVERAGE(O11,N12,O13,P12)</f>
         <v>0.41187871726800618</v>
       </c>
@@ -1725,7 +1744,7 @@
         <f t="shared" ref="Q12" si="68">INDEX($B$2:$E$17,$G12*4+R$1+1,1)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="4">
         <f t="shared" ref="R12" si="69">AVERAGE(R11,Q12,R13,S12)</f>
         <v>0</v>
       </c>
@@ -1733,8 +1752,9 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="12"/>
         <v>12</v>
@@ -1779,11 +1799,12 @@
         <f t="shared" ref="R13" si="73">INDEX($B$2:$E$17,$G12*4+R$1+1,2)</f>
         <v>0</v>
       </c>
-      <c r="S13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="12"/>
         <v>13</v>
@@ -1804,8 +1825,22 @@
         <f>VALUE(paste_here!P14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="12"/>
         <v>14</v>
@@ -1827,7 +1862,7 @@
         <v>0.12983424973188601</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="12"/>
         <v>15</v>

</xml_diff>